<commit_message>
1st push of padj<0.01 results
</commit_message>
<xml_diff>
--- a/GSE107451/processed_data/DESeq_result/DESeq_w1118_male_30_vs_3.xlsx
+++ b/GSE107451/processed_data/DESeq_result/DESeq_w1118_male_30_vs_3.xlsx
@@ -8863,7 +8863,7 @@
         <v>0.0100169808814997</v>
       </c>
       <c r="H66" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67">
@@ -8941,7 +8941,7 @@
         <v>0.0102025226440686</v>
       </c>
       <c r="H69" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70">
@@ -8967,7 +8967,7 @@
         <v>0.0102025226440686</v>
       </c>
       <c r="H70" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71">
@@ -8993,7 +8993,7 @@
         <v>0.0102641768249126</v>
       </c>
       <c r="H71" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72">
@@ -9019,7 +9019,7 @@
         <v>0.0103570349066745</v>
       </c>
       <c r="H72" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73">
@@ -9045,7 +9045,7 @@
         <v>0.0112941606262526</v>
       </c>
       <c r="H73" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74">
@@ -9071,7 +9071,7 @@
         <v>0.0114625054519255</v>
       </c>
       <c r="H74" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75">
@@ -9097,7 +9097,7 @@
         <v>0.0114625054519255</v>
       </c>
       <c r="H75" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76">
@@ -9123,7 +9123,7 @@
         <v>0.0115214600302724</v>
       </c>
       <c r="H76" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77">
@@ -9149,7 +9149,7 @@
         <v>0.0127674156523988</v>
       </c>
       <c r="H77" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78">
@@ -9175,7 +9175,7 @@
         <v>0.0132091444399661</v>
       </c>
       <c r="H78" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79">
@@ -9201,7 +9201,7 @@
         <v>0.0132091444399661</v>
       </c>
       <c r="H79" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80">
@@ -9253,7 +9253,7 @@
         <v>0.0148753745491292</v>
       </c>
       <c r="H81" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82">
@@ -9305,7 +9305,7 @@
         <v>0.0153663822561711</v>
       </c>
       <c r="H83" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="84">
@@ -9331,7 +9331,7 @@
         <v>0.0154775462578889</v>
       </c>
       <c r="H84" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85">
@@ -9357,7 +9357,7 @@
         <v>0.0173138730058547</v>
       </c>
       <c r="H85" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="86">
@@ -9383,7 +9383,7 @@
         <v>0.0176903760470247</v>
       </c>
       <c r="H86" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87">
@@ -9409,7 +9409,7 @@
         <v>0.0187927240350916</v>
       </c>
       <c r="H87" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88">
@@ -9435,7 +9435,7 @@
         <v>0.019205186905548</v>
       </c>
       <c r="H88" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="89">
@@ -9513,7 +9513,7 @@
         <v>0.019648593765767</v>
       </c>
       <c r="H91" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92">
@@ -9539,7 +9539,7 @@
         <v>0.0202019087937496</v>
       </c>
       <c r="H92" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93">
@@ -9565,7 +9565,7 @@
         <v>0.0205774584188853</v>
       </c>
       <c r="H93" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94">
@@ -9669,7 +9669,7 @@
         <v>0.0236765158771312</v>
       </c>
       <c r="H97" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98">
@@ -9695,7 +9695,7 @@
         <v>0.0241180143842227</v>
       </c>
       <c r="H98" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="99">
@@ -9721,7 +9721,7 @@
         <v>0.0258659985659489</v>
       </c>
       <c r="H99" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100">
@@ -9747,7 +9747,7 @@
         <v>0.0258659985659489</v>
       </c>
       <c r="H100" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101">
@@ -9773,7 +9773,7 @@
         <v>0.0263904663188875</v>
       </c>
       <c r="H101" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102">
@@ -9799,7 +9799,7 @@
         <v>0.0270475009491688</v>
       </c>
       <c r="H102" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="103">
@@ -9929,7 +9929,7 @@
         <v>0.0336269679932953</v>
       </c>
       <c r="H107" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="108">
@@ -9981,7 +9981,7 @@
         <v>0.0354657007474372</v>
       </c>
       <c r="H109" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="110">
@@ -10007,7 +10007,7 @@
         <v>0.0365666995648876</v>
       </c>
       <c r="H110" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="111">
@@ -10111,7 +10111,7 @@
         <v>0.0374752855109139</v>
       </c>
       <c r="H114" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="115">
@@ -10163,7 +10163,7 @@
         <v>0.0380753581905178</v>
       </c>
       <c r="H116" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="117">
@@ -10215,7 +10215,7 @@
         <v>0.0395715465694936</v>
       </c>
       <c r="H118" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="119">
@@ -10293,7 +10293,7 @@
         <v>0.0395715465694936</v>
       </c>
       <c r="H121" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="122">
@@ -10319,7 +10319,7 @@
         <v>0.0395715465694936</v>
       </c>
       <c r="H122" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="123">
@@ -10345,7 +10345,7 @@
         <v>0.0395715465694936</v>
       </c>
       <c r="H123" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="124">
@@ -10371,7 +10371,7 @@
         <v>0.0397335647578126</v>
       </c>
       <c r="H124" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="125">
@@ -10423,7 +10423,7 @@
         <v>0.040152952749725</v>
       </c>
       <c r="H126" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="127">
@@ -10449,7 +10449,7 @@
         <v>0.0406368471628554</v>
       </c>
       <c r="H127" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="128">
@@ -10501,7 +10501,7 @@
         <v>0.0406368471628554</v>
       </c>
       <c r="H129" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="130">
@@ -10527,7 +10527,7 @@
         <v>0.0406931177118976</v>
       </c>
       <c r="H130" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="131">
@@ -10553,7 +10553,7 @@
         <v>0.0413081157242968</v>
       </c>
       <c r="H131" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="132">
@@ -10579,7 +10579,7 @@
         <v>0.0415656476411402</v>
       </c>
       <c r="H132" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="133">
@@ -10631,7 +10631,7 @@
         <v>0.0431134203765926</v>
       </c>
       <c r="H134" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="135">
@@ -10657,7 +10657,7 @@
         <v>0.0456904743304524</v>
       </c>
       <c r="H135" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="136">
@@ -10683,7 +10683,7 @@
         <v>0.0456904743304524</v>
       </c>
       <c r="H136" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="137">
@@ -10735,7 +10735,7 @@
         <v>0.0457735994620814</v>
       </c>
       <c r="H138" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="139">
@@ -10761,7 +10761,7 @@
         <v>0.0458323732175925</v>
       </c>
       <c r="H139" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="140">
@@ -10813,7 +10813,7 @@
         <v>0.0464802293322069</v>
       </c>
       <c r="H141" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="142">
@@ -10839,7 +10839,7 @@
         <v>0.0485445998929806</v>
       </c>
       <c r="H142" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="143">
@@ -10865,7 +10865,7 @@
         <v>0.0488391326345506</v>
       </c>
       <c r="H143" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="144">
@@ -10891,7 +10891,7 @@
         <v>0.0492241201578221</v>
       </c>
       <c r="H144" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="145">
@@ -10943,7 +10943,7 @@
         <v>0.0521961900697863</v>
       </c>
       <c r="H146" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="147">
@@ -11021,7 +11021,7 @@
         <v>0.0569279068415471</v>
       </c>
       <c r="H149" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="150">
@@ -11047,7 +11047,7 @@
         <v>0.0569279068415471</v>
       </c>
       <c r="H150" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="151">
@@ -11073,7 +11073,7 @@
         <v>0.0581032033310768</v>
       </c>
       <c r="H151" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="152">
@@ -11099,7 +11099,7 @@
         <v>0.06025467210535</v>
       </c>
       <c r="H152" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="153">
@@ -11151,7 +11151,7 @@
         <v>0.0655217848159662</v>
       </c>
       <c r="H154" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="155">
@@ -11177,7 +11177,7 @@
         <v>0.0669051993052452</v>
       </c>
       <c r="H155" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156">
@@ -11229,7 +11229,7 @@
         <v>0.0684406592777457</v>
       </c>
       <c r="H157" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="158">
@@ -11255,7 +11255,7 @@
         <v>0.0685467060236676</v>
       </c>
       <c r="H158" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="159">
@@ -11333,7 +11333,7 @@
         <v>0.0751141831540064</v>
       </c>
       <c r="H161" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="162">
@@ -11359,7 +11359,7 @@
         <v>0.0768514059299079</v>
       </c>
       <c r="H162" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="163">
@@ -11385,7 +11385,7 @@
         <v>0.0768514059299079</v>
       </c>
       <c r="H163" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="164">
@@ -11463,7 +11463,7 @@
         <v>0.0785598498239345</v>
       </c>
       <c r="H166" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="167">
@@ -11515,7 +11515,7 @@
         <v>0.0789034973879311</v>
       </c>
       <c r="H168" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="169">
@@ -11619,7 +11619,7 @@
         <v>0.0841558896950725</v>
       </c>
       <c r="H172" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="173">
@@ -11671,7 +11671,7 @@
         <v>0.0866484163659492</v>
       </c>
       <c r="H174" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="175">
@@ -11879,7 +11879,7 @@
         <v>0.0901547793116764</v>
       </c>
       <c r="H182" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="183">
@@ -12009,7 +12009,7 @@
         <v>0.097164440992014</v>
       </c>
       <c r="H187" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="188">
@@ -12139,7 +12139,7 @@
         <v>0.0979488839955833</v>
       </c>
       <c r="H192" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="193">
@@ -12165,7 +12165,7 @@
         <v>0.0985268108375842</v>
       </c>
       <c r="H193" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="194">
@@ -12191,7 +12191,7 @@
         <v>0.0985268108375842</v>
       </c>
       <c r="H194" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="195">
@@ -12217,7 +12217,7 @@
         <v>0.0987680163569571</v>
       </c>
       <c r="H195" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="196">
@@ -12243,7 +12243,7 @@
         <v>0.0996216460813885</v>
       </c>
       <c r="H196" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="197">
@@ -12477,7 +12477,7 @@
         <v>0.11504799681734</v>
       </c>
       <c r="H205" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="206">
@@ -12503,7 +12503,7 @@
         <v>0.115335102722009</v>
       </c>
       <c r="H206" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="207">
@@ -12711,7 +12711,7 @@
         <v>0.129067245042411</v>
       </c>
       <c r="H214" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="215">
@@ -12815,7 +12815,7 @@
         <v>0.136186618944209</v>
       </c>
       <c r="H218" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="219">
@@ -12841,7 +12841,7 @@
         <v>0.136186618944209</v>
       </c>
       <c r="H219" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="220">
@@ -12867,7 +12867,7 @@
         <v>0.136858633230629</v>
       </c>
       <c r="H220" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="221">
@@ -12997,7 +12997,7 @@
         <v>0.142805588331918</v>
       </c>
       <c r="H225" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="226">
@@ -13023,7 +13023,7 @@
         <v>0.142805588331918</v>
       </c>
       <c r="H226" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="227">
@@ -13075,7 +13075,7 @@
         <v>0.143913408702533</v>
       </c>
       <c r="H228" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="229">
@@ -13205,7 +13205,7 @@
         <v>0.150596340949763</v>
       </c>
       <c r="H233" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="234">
@@ -13231,7 +13231,7 @@
         <v>0.150953213895306</v>
       </c>
       <c r="H234" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="235">
@@ -13439,7 +13439,7 @@
         <v>0.165625299088992</v>
       </c>
       <c r="H242" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="243">
@@ -13569,7 +13569,7 @@
         <v>0.16997233833362</v>
       </c>
       <c r="H247" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="248">
@@ -13647,7 +13647,7 @@
         <v>0.171827188340121</v>
       </c>
       <c r="H250" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="251">
@@ -13777,7 +13777,7 @@
         <v>0.178050305071064</v>
       </c>
       <c r="H255" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="256">
@@ -13803,7 +13803,7 @@
         <v>0.178050305071064</v>
       </c>
       <c r="H256" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="257">
@@ -13829,7 +13829,7 @@
         <v>0.178243016908791</v>
       </c>
       <c r="H257" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="258">
@@ -13855,7 +13855,7 @@
         <v>0.178243016908791</v>
       </c>
       <c r="H258" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="259">
@@ -13985,7 +13985,7 @@
         <v>0.184605065897931</v>
       </c>
       <c r="H263" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="264">
@@ -14063,7 +14063,7 @@
         <v>0.184782703620036</v>
       </c>
       <c r="H266" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="267">
@@ -14245,7 +14245,7 @@
         <v>0.188354296049199</v>
       </c>
       <c r="H273" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="274">
@@ -14349,7 +14349,7 @@
         <v>0.196295567255728</v>
       </c>
       <c r="H277" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="278">
@@ -14453,7 +14453,7 @@
         <v>0.198997677833353</v>
       </c>
       <c r="H281" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="282">
@@ -14479,7 +14479,7 @@
         <v>0.198997677833353</v>
       </c>
       <c r="H282" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="283">
@@ -14531,7 +14531,7 @@
         <v>0.20131919696601</v>
       </c>
       <c r="H284" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="285">
@@ -14557,7 +14557,7 @@
         <v>0.201741156565475</v>
       </c>
       <c r="H285" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="286">
@@ -14635,7 +14635,7 @@
         <v>0.201741156565475</v>
       </c>
       <c r="H288" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="289">
@@ -14739,7 +14739,7 @@
         <v>0.204263015539605</v>
       </c>
       <c r="H292" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="293">
@@ -14843,7 +14843,7 @@
         <v>0.210203256699412</v>
       </c>
       <c r="H296" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="297">
@@ -15103,7 +15103,7 @@
         <v>0.214698210057538</v>
       </c>
       <c r="H306" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="307">
@@ -15129,7 +15129,7 @@
         <v>0.215261814375362</v>
       </c>
       <c r="H307" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="308">
@@ -15155,7 +15155,7 @@
         <v>0.215261814375362</v>
       </c>
       <c r="H308" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="309">
@@ -15207,7 +15207,7 @@
         <v>0.215261814375362</v>
       </c>
       <c r="H310" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="311">
@@ -15233,7 +15233,7 @@
         <v>0.215541801584479</v>
       </c>
       <c r="H311" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="312">
@@ -15363,7 +15363,7 @@
         <v>0.226570436146329</v>
       </c>
       <c r="H316" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="317">
@@ -15675,7 +15675,7 @@
         <v>0.23868165503243</v>
       </c>
       <c r="H328" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="329">
@@ -15701,7 +15701,7 @@
         <v>0.23868165503243</v>
       </c>
       <c r="H329" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="330">
@@ -15727,7 +15727,7 @@
         <v>0.23868165503243</v>
       </c>
       <c r="H330" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="331">
@@ -15753,7 +15753,7 @@
         <v>0.243697104971997</v>
       </c>
       <c r="H331" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="332">
@@ -15883,7 +15883,7 @@
         <v>0.251414642584967</v>
       </c>
       <c r="H336" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="337">
@@ -15961,7 +15961,7 @@
         <v>0.255133102424966</v>
       </c>
       <c r="H339" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="340">
@@ -16065,7 +16065,7 @@
         <v>0.262239714398409</v>
       </c>
       <c r="H343" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="344">
@@ -16351,7 +16351,7 @@
         <v>0.276189555511952</v>
       </c>
       <c r="H354" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="355">
@@ -16403,7 +16403,7 @@
         <v>0.277674220646159</v>
       </c>
       <c r="H356" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="357">
@@ -16481,7 +16481,7 @@
         <v>0.284356339957874</v>
       </c>
       <c r="H359" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="360">
@@ -16767,7 +16767,7 @@
         <v>0.301449659865222</v>
       </c>
       <c r="H370" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="371">

</xml_diff>